<commit_message>
Apna College Placement Question on Array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimitpanchal/Desktop/CP/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2070D2-E7CE-924D-BAD1-6651A87CAE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="472">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,13 +1420,34 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>Tech Dose</t>
+  </si>
+  <si>
+    <t>Striver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aditya verma </t>
+  </si>
+  <si>
+    <t>Anuj Sharma</t>
+  </si>
+  <si>
+    <t>Better</t>
+  </si>
+  <si>
+    <t>optimal</t>
+  </si>
+  <si>
+    <t>brute force - First solution which comes to the mind</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1855,30 +1870,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:C492"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1889,12 +1904,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1916,7 +1931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1927,7 +1942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1938,7 +1953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21">
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1949,7 +1964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -1960,7 +1975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21">
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1982,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21">
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21">
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2015,7 +2030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21">
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2026,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21">
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2037,7 +2052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21">
+    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2048,7 +2063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2059,7 +2074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2070,7 +2085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21">
+    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2081,7 +2096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21">
+    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2092,7 +2107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21">
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21">
+    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2114,7 +2129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21">
+    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2125,7 +2140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21">
+    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2136,7 +2151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21">
+    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -2147,7 +2162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21">
+    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -2158,7 +2173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21">
+    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -2169,7 +2184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21">
+    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21">
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
@@ -2191,7 +2206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21">
+    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -2202,7 +2217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21">
+    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2213,7 +2228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21">
+    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
@@ -2224,7 +2239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21">
+    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -2235,7 +2250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21">
+    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
@@ -2246,7 +2261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21">
+    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -2257,7 +2272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -2268,7 +2283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21">
+    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -2279,7 +2294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21">
+    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>5</v>
       </c>
@@ -2290,20 +2305,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21">
+    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21">
+    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21">
+    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2314,7 +2329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21">
+    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -2325,7 +2340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21">
+    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
@@ -2336,7 +2351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21">
+    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -2347,7 +2362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21">
+    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>42</v>
       </c>
@@ -2358,7 +2373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21">
+    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2369,7 +2384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21">
+    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>42</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21">
+    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>42</v>
       </c>
@@ -2391,7 +2406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21">
+    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
@@ -2402,7 +2417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21">
+    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>42</v>
       </c>
@@ -2413,12 +2428,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21">
+    <row r="55" spans="1:3" ht="20" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="7"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="21">
+    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -2429,7 +2443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21">
+    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -2440,7 +2454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21">
+    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -2451,7 +2465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21">
+    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -2462,7 +2476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21">
+    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
@@ -2473,7 +2487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21">
+    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
@@ -2484,7 +2498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21">
+    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>53</v>
       </c>
@@ -2495,7 +2509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21">
+    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>53</v>
       </c>
@@ -2506,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21">
+    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>
@@ -2517,7 +2531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="21">
+    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>53</v>
       </c>
@@ -2528,7 +2542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="21">
+    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>53</v>
       </c>
@@ -2539,7 +2553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="21">
+    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
@@ -2550,7 +2564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="21">
+    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
@@ -2561,7 +2575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="21">
+    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>53</v>
       </c>
@@ -2572,7 +2586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="21">
+    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
@@ -2583,7 +2597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="21">
+    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -2594,7 +2608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="21">
+    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
@@ -2605,7 +2619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="21">
+    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -2616,7 +2630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="21">
+    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>53</v>
       </c>
@@ -2627,7 +2641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="21">
+    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
@@ -2638,7 +2652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="21">
+    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
@@ -2649,7 +2663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="21">
+    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -2660,7 +2674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="21">
+    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>53</v>
       </c>
@@ -2671,7 +2685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="21">
+    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>53</v>
       </c>
@@ -2682,7 +2696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="21">
+    <row r="80" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>53</v>
       </c>
@@ -2693,7 +2707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="21">
+    <row r="81" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
@@ -2704,7 +2718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="21">
+    <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>53</v>
       </c>
@@ -2715,7 +2729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="21">
+    <row r="83" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>53</v>
       </c>
@@ -2726,7 +2740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="21">
+    <row r="84" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>53</v>
       </c>
@@ -2737,7 +2751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="21">
+    <row r="85" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>53</v>
       </c>
@@ -2748,7 +2762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="21">
+    <row r="86" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>53</v>
       </c>
@@ -2759,7 +2773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="21">
+    <row r="87" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>53</v>
       </c>
@@ -2770,7 +2784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="21">
+    <row r="88" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>53</v>
       </c>
@@ -2781,7 +2795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="21">
+    <row r="89" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>53</v>
       </c>
@@ -2792,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="21">
+    <row r="90" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>53</v>
       </c>
@@ -2803,7 +2817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="21">
+    <row r="91" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>53</v>
       </c>
@@ -2814,7 +2828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="21">
+    <row r="92" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>53</v>
       </c>
@@ -2825,7 +2839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="21">
+    <row r="93" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>53</v>
       </c>
@@ -2836,7 +2850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="21">
+    <row r="94" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>53</v>
       </c>
@@ -2847,7 +2861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="21">
+    <row r="95" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>53</v>
       </c>
@@ -2858,7 +2872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="21">
+    <row r="96" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>53</v>
       </c>
@@ -2869,7 +2883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="21">
+    <row r="97" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>53</v>
       </c>
@@ -2880,7 +2894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="21">
+    <row r="98" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>53</v>
       </c>
@@ -2891,12 +2905,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="21">
+    <row r="100" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="7"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="21">
+    <row r="101" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>97</v>
       </c>
@@ -2907,7 +2921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="21">
+    <row r="102" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>97</v>
       </c>
@@ -2918,7 +2932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="21">
+    <row r="103" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -2929,7 +2943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="21">
+    <row r="104" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>97</v>
       </c>
@@ -2940,7 +2954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="21">
+    <row r="105" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>97</v>
       </c>
@@ -2951,7 +2965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="21">
+    <row r="106" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>97</v>
       </c>
@@ -2962,7 +2976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="21">
+    <row r="107" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>97</v>
       </c>
@@ -2973,7 +2987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="21">
+    <row r="108" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
@@ -2984,7 +2998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="21">
+    <row r="109" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>97</v>
       </c>
@@ -2995,7 +3009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="21">
+    <row r="110" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>97</v>
       </c>
@@ -3006,7 +3020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="21">
+    <row r="111" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>97</v>
       </c>
@@ -3017,7 +3031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="21">
+    <row r="112" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>97</v>
       </c>
@@ -3028,7 +3042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="21">
+    <row r="113" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>97</v>
       </c>
@@ -3039,7 +3053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="21">
+    <row r="114" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>97</v>
       </c>
@@ -3050,7 +3064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="21">
+    <row r="115" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>97</v>
       </c>
@@ -3061,7 +3075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="21">
+    <row r="116" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>97</v>
       </c>
@@ -3072,7 +3086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="21">
+    <row r="117" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>97</v>
       </c>
@@ -3083,7 +3097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="21">
+    <row r="118" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>97</v>
       </c>
@@ -3094,7 +3108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="21">
+    <row r="119" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>97</v>
       </c>
@@ -3105,7 +3119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="21">
+    <row r="120" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>97</v>
       </c>
@@ -3116,7 +3130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="21">
+    <row r="121" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>97</v>
       </c>
@@ -3127,7 +3141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="21">
+    <row r="122" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>97</v>
       </c>
@@ -3138,7 +3152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="21">
+    <row r="123" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>97</v>
       </c>
@@ -3149,7 +3163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="21">
+    <row r="124" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>97</v>
       </c>
@@ -3160,7 +3174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="21">
+    <row r="125" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>97</v>
       </c>
@@ -3171,7 +3185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="21">
+    <row r="126" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>97</v>
       </c>
@@ -3182,7 +3196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="21">
+    <row r="127" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>97</v>
       </c>
@@ -3193,7 +3207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="21">
+    <row r="128" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>97</v>
       </c>
@@ -3204,7 +3218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="21">
+    <row r="129" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>97</v>
       </c>
@@ -3215,7 +3229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="21">
+    <row r="130" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>97</v>
       </c>
@@ -3226,7 +3240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="21">
+    <row r="131" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>97</v>
       </c>
@@ -3237,7 +3251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="21">
+    <row r="132" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>97</v>
       </c>
@@ -3248,7 +3262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="21">
+    <row r="133" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>97</v>
       </c>
@@ -3259,7 +3273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="21">
+    <row r="134" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>97</v>
       </c>
@@ -3270,7 +3284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="21">
+    <row r="135" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>97</v>
       </c>
@@ -3281,7 +3295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="21">
+    <row r="136" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>97</v>
       </c>
@@ -3292,11 +3306,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="21">
+    <row r="138" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B138" s="7"/>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="1:3" ht="21">
+    <row r="139" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>134</v>
       </c>
@@ -3307,7 +3321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="21">
+    <row r="140" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
         <v>134</v>
       </c>
@@ -3318,7 +3332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="21">
+    <row r="141" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
         <v>134</v>
       </c>
@@ -3329,7 +3343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="21">
+    <row r="142" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
         <v>134</v>
       </c>
@@ -3340,7 +3354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="21">
+    <row r="143" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>134</v>
       </c>
@@ -3351,7 +3365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="21">
+    <row r="144" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
         <v>134</v>
       </c>
@@ -3362,7 +3376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="21">
+    <row r="145" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
         <v>134</v>
       </c>
@@ -3373,7 +3387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="21">
+    <row r="146" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>134</v>
       </c>
@@ -3384,7 +3398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="21">
+    <row r="147" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
         <v>134</v>
       </c>
@@ -3395,7 +3409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="21">
+    <row r="148" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
         <v>134</v>
       </c>
@@ -3406,7 +3420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="21">
+    <row r="149" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
         <v>134</v>
       </c>
@@ -3417,7 +3431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="21">
+    <row r="150" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
         <v>134</v>
       </c>
@@ -3428,7 +3442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="21">
+    <row r="151" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>134</v>
       </c>
@@ -3439,7 +3453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="21">
+    <row r="152" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>134</v>
       </c>
@@ -3450,7 +3464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="21">
+    <row r="153" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>134</v>
       </c>
@@ -3461,7 +3475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="21">
+    <row r="154" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>134</v>
       </c>
@@ -3472,7 +3486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="21">
+    <row r="155" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>134</v>
       </c>
@@ -3483,7 +3497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="21">
+    <row r="156" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>134</v>
       </c>
@@ -3494,7 +3508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="21">
+    <row r="157" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>134</v>
       </c>
@@ -3505,7 +3519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="21">
+    <row r="158" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>134</v>
       </c>
@@ -3516,7 +3530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="21">
+    <row r="159" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>134</v>
       </c>
@@ -3527,7 +3541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="21">
+    <row r="160" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>134</v>
       </c>
@@ -3538,7 +3552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="21">
+    <row r="161" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
         <v>134</v>
       </c>
@@ -3549,7 +3563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="21">
+    <row r="162" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
         <v>134</v>
       </c>
@@ -3560,7 +3574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="21">
+    <row r="163" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
         <v>134</v>
       </c>
@@ -3571,7 +3585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="21">
+    <row r="164" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
         <v>134</v>
       </c>
@@ -3582,7 +3596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="21">
+    <row r="165" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
         <v>134</v>
       </c>
@@ -3593,7 +3607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="21">
+    <row r="166" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
         <v>134</v>
       </c>
@@ -3604,7 +3618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="21">
+    <row r="167" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
         <v>134</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="21">
+    <row r="168" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
         <v>134</v>
       </c>
@@ -3626,7 +3640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="21">
+    <row r="169" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
         <v>134</v>
       </c>
@@ -3637,7 +3651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="21">
+    <row r="170" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
         <v>134</v>
       </c>
@@ -3648,7 +3662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="21">
+    <row r="171" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
         <v>134</v>
       </c>
@@ -3659,7 +3673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="21">
+    <row r="172" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
         <v>134</v>
       </c>
@@ -3670,7 +3684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="21">
+    <row r="173" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
         <v>134</v>
       </c>
@@ -3681,7 +3695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="21">
+    <row r="174" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A174" s="8" t="s">
         <v>134</v>
       </c>
@@ -3692,11 +3706,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="21">
+    <row r="176" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B176" s="7"/>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="1:3" ht="21">
+    <row r="177" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>171</v>
       </c>
@@ -3707,7 +3721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="21">
+    <row r="178" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>171</v>
       </c>
@@ -3718,7 +3732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="21">
+    <row r="179" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>171</v>
       </c>
@@ -3729,7 +3743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="21">
+    <row r="180" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>171</v>
       </c>
@@ -3740,7 +3754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="21">
+    <row r="181" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>171</v>
       </c>
@@ -3751,7 +3765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="21">
+    <row r="182" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>171</v>
       </c>
@@ -3762,7 +3776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="21">
+    <row r="183" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>171</v>
       </c>
@@ -3773,7 +3787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="21">
+    <row r="184" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>171</v>
       </c>
@@ -3784,7 +3798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="21">
+    <row r="185" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>171</v>
       </c>
@@ -3795,7 +3809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="21">
+    <row r="186" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>171</v>
       </c>
@@ -3806,7 +3820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="21">
+    <row r="187" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>171</v>
       </c>
@@ -3817,7 +3831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="21">
+    <row r="188" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>171</v>
       </c>
@@ -3828,7 +3842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="21">
+    <row r="189" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>171</v>
       </c>
@@ -3839,7 +3853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="21">
+    <row r="190" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>171</v>
       </c>
@@ -3850,7 +3864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="21">
+    <row r="191" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>171</v>
       </c>
@@ -3861,7 +3875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="21">
+    <row r="192" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>171</v>
       </c>
@@ -3872,7 +3886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="21">
+    <row r="193" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>171</v>
       </c>
@@ -3883,7 +3897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="21">
+    <row r="194" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>171</v>
       </c>
@@ -3894,7 +3908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="21">
+    <row r="195" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>171</v>
       </c>
@@ -3905,7 +3919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="21">
+    <row r="196" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>171</v>
       </c>
@@ -3916,7 +3930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="21">
+    <row r="197" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -3927,7 +3941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="21">
+    <row r="198" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>171</v>
       </c>
@@ -3938,7 +3952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="21">
+    <row r="199" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>171</v>
       </c>
@@ -3949,7 +3963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="21">
+    <row r="200" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>171</v>
       </c>
@@ -3960,7 +3974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="21">
+    <row r="201" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>171</v>
       </c>
@@ -3971,7 +3985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="21">
+    <row r="202" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>171</v>
       </c>
@@ -3982,7 +3996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="21">
+    <row r="203" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>171</v>
       </c>
@@ -3993,7 +4007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="21">
+    <row r="204" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>171</v>
       </c>
@@ -4004,7 +4018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="21">
+    <row r="205" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>171</v>
       </c>
@@ -4015,7 +4029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="21">
+    <row r="206" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>171</v>
       </c>
@@ -4026,7 +4040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="21">
+    <row r="207" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>171</v>
       </c>
@@ -4037,7 +4051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="21">
+    <row r="208" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>171</v>
       </c>
@@ -4048,7 +4062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="21">
+    <row r="209" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>171</v>
       </c>
@@ -4059,7 +4073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="21">
+    <row r="210" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>171</v>
       </c>
@@ -4070,7 +4084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="21">
+    <row r="211" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>171</v>
       </c>
@@ -4081,17 +4095,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="21">
+    <row r="212" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A212" s="8"/>
       <c r="B212" s="7"/>
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="1:3" ht="21">
+    <row r="213" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A213" s="8"/>
       <c r="B213" s="7"/>
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="1:3" ht="21">
+    <row r="214" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>207</v>
       </c>
@@ -4102,7 +4116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="21">
+    <row r="215" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>207</v>
       </c>
@@ -4113,7 +4127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="21">
+    <row r="216" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>207</v>
       </c>
@@ -4124,7 +4138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="21">
+    <row r="217" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>207</v>
       </c>
@@ -4135,7 +4149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="21">
+    <row r="218" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>207</v>
       </c>
@@ -4146,7 +4160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="21">
+    <row r="219" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>207</v>
       </c>
@@ -4157,7 +4171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="21">
+    <row r="220" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>207</v>
       </c>
@@ -4168,7 +4182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="21">
+    <row r="221" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>207</v>
       </c>
@@ -4179,7 +4193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="21">
+    <row r="222" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>207</v>
       </c>
@@ -4190,7 +4204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="21">
+    <row r="223" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>207</v>
       </c>
@@ -4201,7 +4215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="21">
+    <row r="224" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>207</v>
       </c>
@@ -4212,7 +4226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="21">
+    <row r="225" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>207</v>
       </c>
@@ -4223,7 +4237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="21">
+    <row r="226" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>207</v>
       </c>
@@ -4234,7 +4248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="21">
+    <row r="227" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>207</v>
       </c>
@@ -4245,7 +4259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="21">
+    <row r="228" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>207</v>
       </c>
@@ -4256,7 +4270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="21">
+    <row r="229" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>207</v>
       </c>
@@ -4267,7 +4281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="21">
+    <row r="230" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>207</v>
       </c>
@@ -4278,7 +4292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="21">
+    <row r="231" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>207</v>
       </c>
@@ -4289,7 +4303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="21">
+    <row r="232" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>207</v>
       </c>
@@ -4300,7 +4314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="21">
+    <row r="233" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>207</v>
       </c>
@@ -4311,7 +4325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="21">
+    <row r="234" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>207</v>
       </c>
@@ -4322,7 +4336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="21">
+    <row r="235" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>207</v>
       </c>
@@ -4333,15 +4347,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="21">
+    <row r="236" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B236" s="7"/>
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="1:3" ht="21">
+    <row r="237" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B237" s="7"/>
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="1:3" ht="21">
+    <row r="238" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>230</v>
       </c>
@@ -4352,7 +4366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="21">
+    <row r="239" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>230</v>
       </c>
@@ -4363,7 +4377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="21">
+    <row r="240" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>230</v>
       </c>
@@ -4374,7 +4388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="21">
+    <row r="241" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>230</v>
       </c>
@@ -4385,7 +4399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="21">
+    <row r="242" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
         <v>230</v>
       </c>
@@ -4396,7 +4410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="21">
+    <row r="243" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
         <v>230</v>
       </c>
@@ -4407,7 +4421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="21">
+    <row r="244" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
         <v>230</v>
       </c>
@@ -4418,7 +4432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="21">
+    <row r="245" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
         <v>230</v>
       </c>
@@ -4429,7 +4443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="21">
+    <row r="246" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
         <v>230</v>
       </c>
@@ -4440,7 +4454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="21">
+    <row r="247" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A247" s="5" t="s">
         <v>230</v>
       </c>
@@ -4451,7 +4465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="21">
+    <row r="248" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A248" s="5" t="s">
         <v>230</v>
       </c>
@@ -4462,7 +4476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="21">
+    <row r="249" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A249" s="5" t="s">
         <v>230</v>
       </c>
@@ -4473,7 +4487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="21">
+    <row r="250" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
         <v>230</v>
       </c>
@@ -4484,7 +4498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="21">
+    <row r="251" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
         <v>230</v>
       </c>
@@ -4495,7 +4509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="21">
+    <row r="252" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
         <v>230</v>
       </c>
@@ -4506,7 +4520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="21">
+    <row r="253" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
         <v>230</v>
       </c>
@@ -4517,7 +4531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="21">
+    <row r="254" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
         <v>230</v>
       </c>
@@ -4528,7 +4542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="21">
+    <row r="255" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
         <v>230</v>
       </c>
@@ -4539,7 +4553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="21">
+    <row r="256" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
         <v>230</v>
       </c>
@@ -4550,7 +4564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="21">
+    <row r="257" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A257" s="5" t="s">
         <v>230</v>
       </c>
@@ -4561,7 +4575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="21">
+    <row r="258" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
         <v>230</v>
       </c>
@@ -4572,7 +4586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="21">
+    <row r="259" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A259" s="5" t="s">
         <v>230</v>
       </c>
@@ -4583,7 +4597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="21">
+    <row r="260" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
         <v>230</v>
       </c>
@@ -4594,7 +4608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="21">
+    <row r="261" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
         <v>230</v>
       </c>
@@ -4605,7 +4619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="21">
+    <row r="262" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
         <v>230</v>
       </c>
@@ -4616,7 +4630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="21">
+    <row r="263" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
         <v>230</v>
       </c>
@@ -4627,7 +4641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="21">
+    <row r="264" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
         <v>230</v>
       </c>
@@ -4638,7 +4652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="21">
+    <row r="265" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A265" s="5" t="s">
         <v>230</v>
       </c>
@@ -4649,7 +4663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="21">
+    <row r="266" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
         <v>230</v>
       </c>
@@ -4660,7 +4674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="21">
+    <row r="267" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A267" s="5" t="s">
         <v>230</v>
       </c>
@@ -4671,7 +4685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:3" ht="21">
+    <row r="268" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
         <v>230</v>
       </c>
@@ -4682,7 +4696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="21">
+    <row r="269" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
         <v>230</v>
       </c>
@@ -4693,7 +4707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="21">
+    <row r="270" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
         <v>230</v>
       </c>
@@ -4704,7 +4718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="21">
+    <row r="271" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
         <v>230</v>
       </c>
@@ -4715,7 +4729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="21">
+    <row r="272" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
         <v>230</v>
       </c>
@@ -4726,15 +4740,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="21">
+    <row r="273" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B273" s="7"/>
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="1:3" ht="21">
+    <row r="274" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B274" s="7"/>
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="1:3" ht="21">
+    <row r="275" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A275" s="5" t="s">
         <v>265</v>
       </c>
@@ -4745,7 +4759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="21">
+    <row r="276" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
         <v>265</v>
       </c>
@@ -4756,7 +4770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="21">
+    <row r="277" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
         <v>265</v>
       </c>
@@ -4767,7 +4781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="21">
+    <row r="278" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
         <v>265</v>
       </c>
@@ -4778,7 +4792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="21">
+    <row r="279" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
         <v>265</v>
       </c>
@@ -4789,7 +4803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="21">
+    <row r="280" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A280" s="5" t="s">
         <v>265</v>
       </c>
@@ -4800,7 +4814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="21">
+    <row r="281" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="s">
         <v>265</v>
       </c>
@@ -4811,7 +4825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="21">
+    <row r="282" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
         <v>265</v>
       </c>
@@ -4822,7 +4836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="21">
+    <row r="283" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A283" s="5" t="s">
         <v>265</v>
       </c>
@@ -4833,7 +4847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="21">
+    <row r="284" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
         <v>265</v>
       </c>
@@ -4844,7 +4858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="21">
+    <row r="285" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
         <v>265</v>
       </c>
@@ -4855,7 +4869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="21">
+    <row r="286" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A286" s="5" t="s">
         <v>265</v>
       </c>
@@ -4866,7 +4880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="21">
+    <row r="287" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A287" s="5" t="s">
         <v>265</v>
       </c>
@@ -4877,7 +4891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="21">
+    <row r="288" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
         <v>265</v>
       </c>
@@ -4888,7 +4902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="289" spans="1:3" ht="21">
+    <row r="289" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A289" s="5" t="s">
         <v>265</v>
       </c>
@@ -4899,7 +4913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="290" spans="1:3" ht="21">
+    <row r="290" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
         <v>265</v>
       </c>
@@ -4910,7 +4924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291" spans="1:3" ht="21">
+    <row r="291" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A291" s="5" t="s">
         <v>265</v>
       </c>
@@ -4921,7 +4935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="21">
+    <row r="292" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
         <v>265</v>
       </c>
@@ -4932,7 +4946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:3" ht="21">
+    <row r="293" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A293" s="5" t="s">
         <v>265</v>
       </c>
@@ -4943,15 +4957,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="21">
+    <row r="294" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B294" s="7"/>
       <c r="C294" s="4"/>
     </row>
-    <row r="295" spans="1:3" ht="21">
+    <row r="295" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B295" s="7"/>
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="1:3" ht="21">
+    <row r="296" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
         <v>285</v>
       </c>
@@ -4962,7 +4976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:3" ht="21">
+    <row r="297" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A297" s="5" t="s">
         <v>285</v>
       </c>
@@ -4973,7 +4987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="21">
+    <row r="298" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
         <v>285</v>
       </c>
@@ -4984,7 +4998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="21">
+    <row r="299" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="s">
         <v>285</v>
       </c>
@@ -4995,7 +5009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="21">
+    <row r="300" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
         <v>285</v>
       </c>
@@ -5006,7 +5020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="21">
+    <row r="301" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A301" s="5" t="s">
         <v>285</v>
       </c>
@@ -5017,7 +5031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:3" ht="21">
+    <row r="302" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
         <v>285</v>
       </c>
@@ -5028,7 +5042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="21">
+    <row r="303" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A303" s="5" t="s">
         <v>285</v>
       </c>
@@ -5039,7 +5053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:3" ht="21">
+    <row r="304" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
         <v>285</v>
       </c>
@@ -5050,7 +5064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="21">
+    <row r="305" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A305" s="5" t="s">
         <v>285</v>
       </c>
@@ -5061,7 +5075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="21">
+    <row r="306" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A306" s="5" t="s">
         <v>285</v>
       </c>
@@ -5072,7 +5086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:3" ht="21">
+    <row r="307" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A307" s="5" t="s">
         <v>285</v>
       </c>
@@ -5083,7 +5097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="21">
+    <row r="308" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A308" s="5" t="s">
         <v>285</v>
       </c>
@@ -5094,7 +5108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:3" ht="21">
+    <row r="309" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A309" s="5" t="s">
         <v>285</v>
       </c>
@@ -5105,7 +5119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="310" spans="1:3" ht="21">
+    <row r="310" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
         <v>285</v>
       </c>
@@ -5116,7 +5130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:3" ht="21">
+    <row r="311" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A311" s="5" t="s">
         <v>285</v>
       </c>
@@ -5127,7 +5141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:3" ht="21">
+    <row r="312" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
         <v>285</v>
       </c>
@@ -5138,7 +5152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="313" spans="1:3" ht="21">
+    <row r="313" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A313" s="5" t="s">
         <v>285</v>
       </c>
@@ -5149,7 +5163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="314" spans="1:3" ht="21">
+    <row r="314" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
         <v>285</v>
       </c>
@@ -5160,7 +5174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="315" spans="1:3" ht="21">
+    <row r="315" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
         <v>285</v>
       </c>
@@ -5171,7 +5185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="316" spans="1:3" ht="21">
+    <row r="316" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
         <v>285</v>
       </c>
@@ -5182,7 +5196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="317" spans="1:3" ht="21">
+    <row r="317" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A317" s="5" t="s">
         <v>285</v>
       </c>
@@ -5193,7 +5207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:3" ht="21">
+    <row r="318" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A318" s="5" t="s">
         <v>285</v>
       </c>
@@ -5204,7 +5218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:3" ht="21">
+    <row r="319" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A319" s="5" t="s">
         <v>285</v>
       </c>
@@ -5215,7 +5229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:3" ht="21">
+    <row r="320" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A320" s="5" t="s">
         <v>285</v>
       </c>
@@ -5226,7 +5240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="321" spans="1:3" ht="21">
+    <row r="321" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A321" s="5" t="s">
         <v>285</v>
       </c>
@@ -5237,7 +5251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="322" spans="1:3" ht="21">
+    <row r="322" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A322" s="5" t="s">
         <v>285</v>
       </c>
@@ -5248,7 +5262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="21">
+    <row r="323" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A323" s="5" t="s">
         <v>285</v>
       </c>
@@ -5259,7 +5273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="324" spans="1:3" ht="21">
+    <row r="324" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A324" s="5" t="s">
         <v>285</v>
       </c>
@@ -5270,7 +5284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="325" spans="1:3" ht="21">
+    <row r="325" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A325" s="5" t="s">
         <v>285</v>
       </c>
@@ -5281,7 +5295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:3" ht="21">
+    <row r="326" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A326" s="5" t="s">
         <v>285</v>
       </c>
@@ -5292,7 +5306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:3" ht="21">
+    <row r="327" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A327" s="5" t="s">
         <v>285</v>
       </c>
@@ -5303,7 +5317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="328" spans="1:3" ht="21">
+    <row r="328" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A328" s="5" t="s">
         <v>285</v>
       </c>
@@ -5314,7 +5328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="21">
+    <row r="329" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A329" s="5" t="s">
         <v>285</v>
       </c>
@@ -5325,7 +5339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="330" spans="1:3" ht="21">
+    <row r="330" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A330" s="5" t="s">
         <v>285</v>
       </c>
@@ -5336,7 +5350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="331" spans="1:3" ht="21">
+    <row r="331" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A331" s="5" t="s">
         <v>285</v>
       </c>
@@ -5347,7 +5361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="332" spans="1:3" ht="21">
+    <row r="332" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A332" s="5" t="s">
         <v>285</v>
       </c>
@@ -5358,7 +5372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:3" ht="21">
+    <row r="333" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A333" s="5" t="s">
         <v>285</v>
       </c>
@@ -5369,15 +5383,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="334" spans="1:3" ht="21">
+    <row r="334" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B334" s="7"/>
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="1:3" ht="21">
+    <row r="335" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B335" s="7"/>
       <c r="C335" s="4"/>
     </row>
-    <row r="336" spans="1:3" ht="21">
+    <row r="336" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A336" s="8" t="s">
         <v>324</v>
       </c>
@@ -5388,7 +5402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="337" spans="1:3" ht="21">
+    <row r="337" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A337" s="8" t="s">
         <v>324</v>
       </c>
@@ -5399,7 +5413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:3" ht="21">
+    <row r="338" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A338" s="8" t="s">
         <v>324</v>
       </c>
@@ -5410,7 +5424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="339" spans="1:3" ht="21">
+    <row r="339" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A339" s="8" t="s">
         <v>324</v>
       </c>
@@ -5421,7 +5435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="21">
+    <row r="340" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A340" s="8" t="s">
         <v>324</v>
       </c>
@@ -5432,7 +5446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="341" spans="1:3" ht="21">
+    <row r="341" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A341" s="8" t="s">
         <v>324</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="21">
+    <row r="342" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A342" s="8" t="s">
         <v>324</v>
       </c>
@@ -5454,7 +5468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="343" spans="1:3" ht="21">
+    <row r="343" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A343" s="8" t="s">
         <v>324</v>
       </c>
@@ -5465,7 +5479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="21">
+    <row r="344" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A344" s="8" t="s">
         <v>324</v>
       </c>
@@ -5476,7 +5490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:3" ht="21">
+    <row r="345" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A345" s="8" t="s">
         <v>324</v>
       </c>
@@ -5487,7 +5501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:3" ht="21">
+    <row r="346" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A346" s="8" t="s">
         <v>324</v>
       </c>
@@ -5498,7 +5512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:3" ht="21">
+    <row r="347" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A347" s="8" t="s">
         <v>324</v>
       </c>
@@ -5509,7 +5523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="348" spans="1:3" ht="21">
+    <row r="348" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A348" s="8" t="s">
         <v>324</v>
       </c>
@@ -5520,7 +5534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="21">
+    <row r="349" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A349" s="8" t="s">
         <v>324</v>
       </c>
@@ -5531,7 +5545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:3" ht="21">
+    <row r="350" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A350" s="8" t="s">
         <v>324</v>
       </c>
@@ -5542,7 +5556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="21">
+    <row r="351" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A351" s="8" t="s">
         <v>324</v>
       </c>
@@ -5553,7 +5567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:3" ht="21">
+    <row r="352" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A352" s="8" t="s">
         <v>324</v>
       </c>
@@ -5564,7 +5578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:3" ht="21">
+    <row r="353" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A353" s="8" t="s">
         <v>324</v>
       </c>
@@ -5575,15 +5589,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="354" spans="1:3" ht="21">
+    <row r="354" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B354" s="7"/>
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="1:3" ht="21">
+    <row r="355" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B355" s="7"/>
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="1:3" ht="21">
+    <row r="356" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A356" s="8" t="s">
         <v>343</v>
       </c>
@@ -5594,7 +5608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="357" spans="1:3" ht="21">
+    <row r="357" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A357" s="8" t="s">
         <v>343</v>
       </c>
@@ -5605,7 +5619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="358" spans="1:3" ht="21">
+    <row r="358" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A358" s="8" t="s">
         <v>343</v>
       </c>
@@ -5616,7 +5630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="359" spans="1:3" ht="21">
+    <row r="359" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A359" s="8" t="s">
         <v>343</v>
       </c>
@@ -5627,7 +5641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="360" spans="1:3" ht="21">
+    <row r="360" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A360" s="8" t="s">
         <v>343</v>
       </c>
@@ -5638,7 +5652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="361" spans="1:3" ht="21">
+    <row r="361" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A361" s="8" t="s">
         <v>343</v>
       </c>
@@ -5649,7 +5663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="362" spans="1:3" ht="21">
+    <row r="362" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A362" s="8" t="s">
         <v>343</v>
       </c>
@@ -5660,7 +5674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="21">
+    <row r="363" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A363" s="8" t="s">
         <v>343</v>
       </c>
@@ -5671,7 +5685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="364" spans="1:3" ht="21">
+    <row r="364" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A364" s="8" t="s">
         <v>343</v>
       </c>
@@ -5682,7 +5696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="365" spans="1:3" ht="21">
+    <row r="365" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A365" s="8" t="s">
         <v>343</v>
       </c>
@@ -5693,7 +5707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="366" spans="1:3" ht="21">
+    <row r="366" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A366" s="8" t="s">
         <v>343</v>
       </c>
@@ -5704,7 +5718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="367" spans="1:3" ht="21">
+    <row r="367" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A367" s="8" t="s">
         <v>343</v>
       </c>
@@ -5715,7 +5729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:3" ht="21">
+    <row r="368" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A368" s="8" t="s">
         <v>343</v>
       </c>
@@ -5726,7 +5740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="369" spans="1:3" ht="21">
+    <row r="369" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A369" s="8" t="s">
         <v>343</v>
       </c>
@@ -5737,7 +5751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="370" spans="1:3" ht="21">
+    <row r="370" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A370" s="8" t="s">
         <v>343</v>
       </c>
@@ -5748,7 +5762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="371" spans="1:3" ht="21">
+    <row r="371" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A371" s="8" t="s">
         <v>343</v>
       </c>
@@ -5759,7 +5773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="372" spans="1:3" ht="21">
+    <row r="372" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A372" s="8" t="s">
         <v>343</v>
       </c>
@@ -5770,7 +5784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="373" spans="1:3" ht="21">
+    <row r="373" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A373" s="8" t="s">
         <v>343</v>
       </c>
@@ -5781,7 +5795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="374" spans="1:3" ht="21">
+    <row r="374" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A374" s="8" t="s">
         <v>343</v>
       </c>
@@ -5792,7 +5806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="375" spans="1:3" ht="21">
+    <row r="375" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A375" s="8" t="s">
         <v>343</v>
       </c>
@@ -5803,7 +5817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:3" ht="21">
+    <row r="376" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A376" s="8" t="s">
         <v>343</v>
       </c>
@@ -5814,7 +5828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="377" spans="1:3" ht="21">
+    <row r="377" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A377" s="8" t="s">
         <v>343</v>
       </c>
@@ -5825,7 +5839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="378" spans="1:3" ht="21">
+    <row r="378" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A378" s="8" t="s">
         <v>343</v>
       </c>
@@ -5836,7 +5850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="379" spans="1:3" ht="21">
+    <row r="379" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A379" s="8" t="s">
         <v>343</v>
       </c>
@@ -5847,7 +5861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="380" spans="1:3" ht="21">
+    <row r="380" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A380" s="8" t="s">
         <v>343</v>
       </c>
@@ -5858,7 +5872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:3" ht="21">
+    <row r="381" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A381" s="8" t="s">
         <v>343</v>
       </c>
@@ -5869,7 +5883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:3" ht="21">
+    <row r="382" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A382" s="8" t="s">
         <v>343</v>
       </c>
@@ -5880,7 +5894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:3" ht="21">
+    <row r="383" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A383" s="8" t="s">
         <v>343</v>
       </c>
@@ -5891,7 +5905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:3" ht="21">
+    <row r="384" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A384" s="8" t="s">
         <v>343</v>
       </c>
@@ -5902,7 +5916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="385" spans="1:3" ht="21">
+    <row r="385" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A385" s="8" t="s">
         <v>343</v>
       </c>
@@ -5913,7 +5927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:3" ht="21">
+    <row r="386" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A386" s="8" t="s">
         <v>343</v>
       </c>
@@ -5924,7 +5938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="21">
+    <row r="387" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A387" s="8" t="s">
         <v>343</v>
       </c>
@@ -5935,7 +5949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:3" ht="21">
+    <row r="388" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A388" s="8" t="s">
         <v>343</v>
       </c>
@@ -5946,7 +5960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="21">
+    <row r="389" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A389" s="8" t="s">
         <v>343</v>
       </c>
@@ -5957,7 +5971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="21">
+    <row r="390" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A390" s="8" t="s">
         <v>343</v>
       </c>
@@ -5968,7 +5982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="391" spans="1:3" ht="21">
+    <row r="391" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A391" s="8" t="s">
         <v>343</v>
       </c>
@@ -5979,7 +5993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:3" ht="21">
+    <row r="392" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A392" s="8" t="s">
         <v>343</v>
       </c>
@@ -5990,7 +6004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="393" spans="1:3" ht="21">
+    <row r="393" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
         <v>343</v>
       </c>
@@ -6001,7 +6015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="394" spans="1:3" ht="21">
+    <row r="394" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A394" s="8" t="s">
         <v>343</v>
       </c>
@@ -6012,7 +6026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="21">
+    <row r="395" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A395" s="8" t="s">
         <v>343</v>
       </c>
@@ -6023,7 +6037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="21">
+    <row r="396" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A396" s="8" t="s">
         <v>343</v>
       </c>
@@ -6034,7 +6048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="21">
+    <row r="397" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A397" s="8" t="s">
         <v>343</v>
       </c>
@@ -6045,7 +6059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="21">
+    <row r="398" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A398" s="8" t="s">
         <v>343</v>
       </c>
@@ -6056,7 +6070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:3" ht="21">
+    <row r="399" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A399" s="8" t="s">
         <v>343</v>
       </c>
@@ -6067,15 +6081,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="21">
-      <c r="B400" s="7"/>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="1:3" ht="21">
-      <c r="B401" s="7"/>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="1:3" ht="21">
+    <row r="402" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A402" s="8" t="s">
         <v>387</v>
       </c>
@@ -6086,7 +6098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="21">
+    <row r="403" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A403" s="8" t="s">
         <v>387</v>
       </c>
@@ -6097,7 +6109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="21">
+    <row r="404" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A404" s="8" t="s">
         <v>387</v>
       </c>
@@ -6108,7 +6120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="21">
+    <row r="405" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A405" s="8" t="s">
         <v>387</v>
       </c>
@@ -6119,7 +6131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="21">
+    <row r="406" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A406" s="8" t="s">
         <v>387</v>
       </c>
@@ -6130,7 +6142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="21">
+    <row r="407" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A407" s="8" t="s">
         <v>387</v>
       </c>
@@ -6141,15 +6153,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="21">
+    <row r="408" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B408" s="7"/>
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="1:3" ht="21">
+    <row r="409" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B409" s="7"/>
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="1:3" ht="21">
+    <row r="410" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A410" s="5" t="s">
         <v>393</v>
       </c>
@@ -6160,7 +6172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="21">
+    <row r="411" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A411" s="5" t="s">
         <v>393</v>
       </c>
@@ -6171,7 +6183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="21">
+    <row r="412" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A412" s="5" t="s">
         <v>393</v>
       </c>
@@ -6182,7 +6194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="21">
+    <row r="413" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A413" s="5" t="s">
         <v>393</v>
       </c>
@@ -6193,7 +6205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="21">
+    <row r="414" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A414" s="5" t="s">
         <v>393</v>
       </c>
@@ -6204,7 +6216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:3" ht="21">
+    <row r="415" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A415" s="5" t="s">
         <v>393</v>
       </c>
@@ -6215,7 +6227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="21">
+    <row r="416" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A416" s="5" t="s">
         <v>393</v>
       </c>
@@ -6226,7 +6238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="21">
+    <row r="417" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A417" s="5" t="s">
         <v>393</v>
       </c>
@@ -6237,7 +6249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="21">
+    <row r="418" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A418" s="5" t="s">
         <v>393</v>
       </c>
@@ -6248,7 +6260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="21">
+    <row r="419" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A419" s="5" t="s">
         <v>393</v>
       </c>
@@ -6259,7 +6271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="21">
+    <row r="420" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A420" s="5" t="s">
         <v>393</v>
       </c>
@@ -6270,7 +6282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:3" ht="21">
+    <row r="421" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A421" s="5" t="s">
         <v>393</v>
       </c>
@@ -6281,7 +6293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:3" ht="21">
+    <row r="422" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A422" s="5" t="s">
         <v>393</v>
       </c>
@@ -6292,7 +6304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:3" ht="21">
+    <row r="423" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A423" s="5" t="s">
         <v>393</v>
       </c>
@@ -6303,7 +6315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="21">
+    <row r="424" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A424" s="5" t="s">
         <v>393</v>
       </c>
@@ -6314,7 +6326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:3" ht="21">
+    <row r="425" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A425" s="5" t="s">
         <v>393</v>
       </c>
@@ -6325,7 +6337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="21">
+    <row r="426" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A426" s="5" t="s">
         <v>393</v>
       </c>
@@ -6336,7 +6348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="21">
+    <row r="427" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A427" s="5" t="s">
         <v>393</v>
       </c>
@@ -6347,7 +6359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="21">
+    <row r="428" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A428" s="5" t="s">
         <v>393</v>
       </c>
@@ -6358,7 +6370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="21">
+    <row r="429" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A429" s="5" t="s">
         <v>393</v>
       </c>
@@ -6369,7 +6381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="21">
+    <row r="430" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A430" s="5" t="s">
         <v>393</v>
       </c>
@@ -6380,7 +6392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="431" spans="1:3" ht="21">
+    <row r="431" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A431" s="5" t="s">
         <v>393</v>
       </c>
@@ -6391,7 +6403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:3" ht="21">
+    <row r="432" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A432" s="5" t="s">
         <v>393</v>
       </c>
@@ -6402,7 +6414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="21">
+    <row r="433" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A433" s="5" t="s">
         <v>393</v>
       </c>
@@ -6413,7 +6425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="21">
+    <row r="434" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A434" s="5" t="s">
         <v>393</v>
       </c>
@@ -6424,7 +6436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="21">
+    <row r="435" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A435" s="5" t="s">
         <v>393</v>
       </c>
@@ -6435,7 +6447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="21">
+    <row r="436" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A436" s="5" t="s">
         <v>393</v>
       </c>
@@ -6446,7 +6458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="21">
+    <row r="437" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A437" s="5" t="s">
         <v>393</v>
       </c>
@@ -6457,7 +6469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:3" ht="21">
+    <row r="438" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A438" s="5" t="s">
         <v>393</v>
       </c>
@@ -6468,7 +6480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="21">
+    <row r="439" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A439" s="5" t="s">
         <v>393</v>
       </c>
@@ -6479,7 +6491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="21">
+    <row r="440" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A440" s="5" t="s">
         <v>393</v>
       </c>
@@ -6490,7 +6502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="441" spans="1:3" ht="21">
+    <row r="441" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A441" s="5" t="s">
         <v>393</v>
       </c>
@@ -6501,7 +6513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="442" spans="1:3" ht="21">
+    <row r="442" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A442" s="5" t="s">
         <v>393</v>
       </c>
@@ -6512,7 +6524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="21">
+    <row r="443" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A443" s="5" t="s">
         <v>393</v>
       </c>
@@ -6523,7 +6535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="21">
+    <row r="444" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A444" s="5" t="s">
         <v>393</v>
       </c>
@@ -6534,7 +6546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="21">
+    <row r="445" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A445" s="5" t="s">
         <v>393</v>
       </c>
@@ -6545,7 +6557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="21">
+    <row r="446" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A446" s="5" t="s">
         <v>393</v>
       </c>
@@ -6556,7 +6568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="447" spans="1:3" ht="21">
+    <row r="447" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A447" s="5" t="s">
         <v>393</v>
       </c>
@@ -6567,7 +6579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:3" ht="21">
+    <row r="448" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A448" s="5" t="s">
         <v>393</v>
       </c>
@@ -6578,7 +6590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="21">
+    <row r="449" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A449" s="5" t="s">
         <v>393</v>
       </c>
@@ -6589,7 +6601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="21">
+    <row r="450" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A450" s="5" t="s">
         <v>393</v>
       </c>
@@ -6600,7 +6612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="451" spans="1:3" ht="21">
+    <row r="451" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A451" s="5" t="s">
         <v>393</v>
       </c>
@@ -6611,7 +6623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="21">
+    <row r="452" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A452" s="5" t="s">
         <v>393</v>
       </c>
@@ -6622,7 +6634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="21">
+    <row r="453" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A453" s="5" t="s">
         <v>393</v>
       </c>
@@ -6633,7 +6645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="21">
+    <row r="454" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A454" s="5" t="s">
         <v>393</v>
       </c>
@@ -6644,7 +6656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="21">
+    <row r="455" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A455" s="5" t="s">
         <v>393</v>
       </c>
@@ -6655,7 +6667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="21">
+    <row r="456" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A456" s="5" t="s">
         <v>393</v>
       </c>
@@ -6666,7 +6678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="21">
+    <row r="457" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A457" s="5" t="s">
         <v>393</v>
       </c>
@@ -6677,7 +6689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="458" spans="1:3" ht="21">
+    <row r="458" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A458" s="5" t="s">
         <v>393</v>
       </c>
@@ -6688,7 +6700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="21">
+    <row r="459" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A459" s="5" t="s">
         <v>393</v>
       </c>
@@ -6699,7 +6711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="460" spans="1:3" ht="21">
+    <row r="460" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A460" s="5" t="s">
         <v>393</v>
       </c>
@@ -6710,7 +6722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="461" spans="1:3" ht="21">
+    <row r="461" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A461" s="5" t="s">
         <v>393</v>
       </c>
@@ -6721,7 +6733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="462" spans="1:3" ht="21">
+    <row r="462" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A462" s="5" t="s">
         <v>393</v>
       </c>
@@ -6732,7 +6744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="463" spans="1:3" ht="21">
+    <row r="463" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A463" s="5" t="s">
         <v>393</v>
       </c>
@@ -6743,7 +6755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="21">
+    <row r="464" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A464" s="5" t="s">
         <v>393</v>
       </c>
@@ -6754,7 +6766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="465" spans="1:3" ht="21">
+    <row r="465" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A465" s="5" t="s">
         <v>393</v>
       </c>
@@ -6765,7 +6777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="466" spans="1:3" ht="21">
+    <row r="466" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A466" s="5" t="s">
         <v>393</v>
       </c>
@@ -6776,7 +6788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="21">
+    <row r="467" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A467" s="5" t="s">
         <v>393</v>
       </c>
@@ -6787,7 +6799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="468" spans="1:3" ht="21">
+    <row r="468" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A468" s="5" t="s">
         <v>393</v>
       </c>
@@ -6798,7 +6810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="469" spans="1:3" ht="21">
+    <row r="469" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A469" s="5" t="s">
         <v>393</v>
       </c>
@@ -6809,16 +6821,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="21">
+    <row r="470" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="B470" s="7"/>
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="1:3" ht="21">
+    <row r="471" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A471" s="8"/>
       <c r="B471" s="7"/>
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="1:3" ht="21">
+    <row r="472" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A472" s="5" t="s">
         <v>453</v>
       </c>
@@ -6829,7 +6841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="473" spans="1:3" ht="21">
+    <row r="473" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A473" s="5" t="s">
         <v>453</v>
       </c>
@@ -6840,7 +6852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="474" spans="1:3" ht="21">
+    <row r="474" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A474" s="5" t="s">
         <v>453</v>
       </c>
@@ -6851,7 +6863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="475" spans="1:3" ht="21">
+    <row r="475" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A475" s="5" t="s">
         <v>453</v>
       </c>
@@ -6862,7 +6874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="476" spans="1:3" ht="21">
+    <row r="476" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A476" s="5" t="s">
         <v>453</v>
       </c>
@@ -6873,7 +6885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="477" spans="1:3" ht="21">
+    <row r="477" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A477" s="5" t="s">
         <v>453</v>
       </c>
@@ -6884,7 +6896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="478" spans="1:3" ht="21">
+    <row r="478" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A478" s="5" t="s">
         <v>453</v>
       </c>
@@ -6895,7 +6907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="479" spans="1:3" ht="21">
+    <row r="479" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A479" s="5" t="s">
         <v>453</v>
       </c>
@@ -6906,7 +6918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="480" spans="1:3" ht="21">
+    <row r="480" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A480" s="5" t="s">
         <v>453</v>
       </c>
@@ -6917,7 +6929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="481" spans="1:3" ht="21">
+    <row r="481" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A481" s="5" t="s">
         <v>453</v>
       </c>
@@ -6926,6 +6938,41 @@
       </c>
       <c r="C481" s="4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B484" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B485" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B486" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B487" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B490" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B491" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B492" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>